<commit_message>
rnc-9/08/2015-se modifico el formato de algunos documentos CP_ADMINISTRARUSUARIO_AFGMX.docx, CP_CONSULTADATOS_AFGMX.docx, CP_INICIOSESION_AFGMX.docx, CP_REGISTRARUSUARIO_AFGMX.docx, PL_CONTROLPRUEBAS_AFGMX.xlsx, PL_PRUEBA.docx, PLAN_DE_PRUEBAS.xlsx) y se agregaron nuevos referentes al plan de pruebas(CP_GENERAR_REPORTE_AFG.docx, CP_GESTIONAR_CULTIVOS.docx, CP_GESTIONAR_DATOS_AFG.docx).
</commit_message>
<xml_diff>
--- a/ afgmx/AFGMX/PROCESO_DESARROLLO/F5_PRUEBAS/PL_PRUEBAS/PLAN_DE_PRUEBAS.xlsx
+++ b/ afgmx/AFGMX/PROCESO_DESARROLLO/F5_PRUEBAS/PL_PRUEBAS/PLAN_DE_PRUEBAS.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\DocumentacionTester\Pruebas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="440"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="440"/>
   </bookViews>
   <sheets>
     <sheet name="Plan de Pruebas" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="50">
   <si>
     <t>PLAN DE PRUEBAS</t>
   </si>
@@ -120,31 +115,55 @@
     <t>Consultar sugerencia de cultivo</t>
   </si>
   <si>
-    <t>CU-006-01</t>
-  </si>
-  <si>
-    <t>CU-006-02</t>
-  </si>
-  <si>
-    <t>CU-006-04</t>
-  </si>
-  <si>
-    <t>CU-006-06</t>
-  </si>
-  <si>
     <t>Implementación del Sistema de Consultas del tipo de suelo</t>
   </si>
   <si>
     <t>CU-002-02</t>
   </si>
   <si>
-    <t>CU-006-07</t>
-  </si>
-  <si>
     <t>Iniciar sesion</t>
   </si>
   <si>
-    <t>Administrar historicos</t>
+    <t>Consultar historicos</t>
+  </si>
+  <si>
+    <t>CU-004-01</t>
+  </si>
+  <si>
+    <t>CU-004-02</t>
+  </si>
+  <si>
+    <t>CU-004-07</t>
+  </si>
+  <si>
+    <t>CU-004-03</t>
+  </si>
+  <si>
+    <t>CU-004-05</t>
+  </si>
+  <si>
+    <t>Gestionar cultivos</t>
+  </si>
+  <si>
+    <t>CU-003-02</t>
+  </si>
+  <si>
+    <t>Generar Reporte</t>
+  </si>
+  <si>
+    <t>CU-003-03</t>
+  </si>
+  <si>
+    <t>Consultar elevaciones</t>
+  </si>
+  <si>
+    <t>CU-004-08</t>
+  </si>
+  <si>
+    <t>CU-004-09</t>
+  </si>
+  <si>
+    <t>Gestionar datos</t>
   </si>
 </sst>
 </file>
@@ -195,7 +214,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -330,17 +349,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF00000A"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF00000A"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF00000A"/>
@@ -365,47 +373,41 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thin">
+        <color rgb="FF00000A"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color rgb="FF00000A"/>
       </right>
       <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -442,86 +444,101 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -613,15 +630,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>538371</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>115956</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1474305</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>15018</xdr:rowOff>
+      <xdr:colOff>670890</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>8282</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -643,8 +660,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="538371" y="115956"/>
-          <a:ext cx="935934" cy="892975"/>
+          <a:off x="0" y="0"/>
+          <a:ext cx="670890" cy="505239"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -660,11 +677,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>66261</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>65413</xdr:rowOff>
+      <xdr:colOff>433288</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>131674</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1973617" cy="374141"/>
+    <xdr:ext cx="726033" cy="387286"/>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="2" name="Rectángulo 1"/>
@@ -672,8 +689,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="66261" y="396717"/>
-          <a:ext cx="1973617" cy="374141"/>
+          <a:off x="433288" y="131674"/>
+          <a:ext cx="726033" cy="387286"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -688,7 +705,7 @@
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="es-ES" sz="1800" b="1" cap="none" spc="0">
+            <a:rPr lang="es-ES" sz="2000" b="1" cap="none" spc="0">
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="bg1"/>
@@ -708,8 +725,10 @@
                   </a:schemeClr>
                 </a:outerShdw>
               </a:effectLst>
+              <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t>AgroFinderGround</a:t>
+            <a:t>AFG</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -762,7 +781,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,7 +816,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1008,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1023,30 +1042,30 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
-      <c r="F5" s="24"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="39"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
@@ -1060,51 +1079,51 @@
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
+      <c r="B9" s="42" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" spans="1:6" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="29"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="19">
+      <c r="B11" s="17">
         <v>42091</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="17">
         <v>42091</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="45" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1112,17 +1131,17 @@
       <c r="A12" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
@@ -1136,13 +1155,13 @@
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="23"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
@@ -1172,7 +1191,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="16">
+      <c r="A17" s="15">
         <v>1</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -1187,16 +1206,16 @@
       <c r="E17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="32">
+      <c r="A18" s="30">
         <v>2</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C18" s="13" t="s">
         <v>25</v>
@@ -1207,17 +1226,17 @@
       <c r="E18" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="18" t="s">
+      <c r="F18" s="16" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="33"/>
+      <c r="A19" s="31"/>
       <c r="B19" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>14</v>
@@ -1225,93 +1244,93 @@
       <c r="E19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F19" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="33">
         <v>3</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F20" s="18" t="s">
+      <c r="F20" s="25" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="38">
+      <c r="A21" s="34"/>
+      <c r="B21" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="34"/>
+      <c r="B22" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="32">
         <v>4</v>
       </c>
-      <c r="B21" s="34" t="s">
+      <c r="B23" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="8" t="s">
+      <c r="C23" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F21" s="18" t="s">
+      <c r="F23" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="39"/>
-      <c r="B22" s="35" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="32"/>
+      <c r="B24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" s="39"/>
-      <c r="B23" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F23" s="18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" s="39"/>
-      <c r="B24" s="36" t="s">
-        <v>30</v>
-      </c>
       <c r="C24" s="13" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>14</v>
@@ -1319,17 +1338,17 @@
       <c r="E24" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
-      <c r="B25" s="36" t="s">
-        <v>31</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="32"/>
+      <c r="B25" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>14</v>
@@ -1337,15 +1356,87 @@
       <c r="E25" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="16" t="s">
         <v>24</v>
       </c>
     </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="32"/>
+      <c r="B26" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="32"/>
+      <c r="B27" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="32"/>
+      <c r="B28" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="37"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="F29" s="29" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A23:A29"/>
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="B14:F14"/>
     <mergeCell ref="A4:F6"/>
     <mergeCell ref="B8:F8"/>
@@ -1353,11 +1444,9 @@
     <mergeCell ref="B9:F10"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="F11:F12"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A21:A25"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D25">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D17:D20 D23:D27">
       <formula1>"Integración, Sistema"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>